<commit_message>
Committing excel with datastructures sheet
</commit_message>
<xml_diff>
--- a/DS_ALGO_PROJECT/src/test/resources/ExcelData/ExcelData.xlsx
+++ b/DS_ALGO_PROJECT/src/test/resources/ExcelData/ExcelData.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6FD7528A-F1F6-47F2-A58C-13921706C35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashok\git\DS-ALGOPROJECT_MAIN\DS_ALGO_PROJECT\src\test\resources\ExcelData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C4D8CF-7436-45FF-92D5-269B72E35DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="DataStructures" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -28,6 +33,12 @@
   </si>
   <si>
     <t>Kind@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("Hello, World!") </t>
+  </si>
+  <si>
+    <t>hello Cool Cukes</t>
   </si>
 </sst>
 </file>
@@ -291,13 +302,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -305,12 +316,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99267A7C-9DCF-44F7-B0AF-BD21629D0982}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the excel with some more python code
</commit_message>
<xml_diff>
--- a/DS_ALGO_PROJECT/src/test/resources/ExcelData/ExcelData.xlsx
+++ b/DS_ALGO_PROJECT/src/test/resources/ExcelData/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashok\git\DS-ALGOPROJECT_MAIN\DS_ALGO_PROJECT\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C4D8CF-7436-45FF-92D5-269B72E35DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCA8156-8468-45BA-8002-591B16F4191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -35,17 +35,102 @@
     <t>Kind@123</t>
   </si>
   <si>
-    <t xml:space="preserve">print("Hello, World!") </t>
-  </si>
-  <si>
-    <t>hello Cool Cukes</t>
+    <t>pythonCode</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>print("hello World");</t>
+  </si>
+  <si>
+    <t>hello cool cukes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -58,13 +143,30 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,9 +181,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,25 +438,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99267A7C-9DCF-44F7-B0AF-BD21629D0982}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>